<commit_message>
changes in step 2 of prop grantt 23-24
</commit_message>
<xml_diff>
--- a/tab_car_licit_illicit_2.xlsx
+++ b/tab_car_licit_illicit_2.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="321">
   <si>
     <t xml:space="preserve">characteristic</t>
   </si>
   <si>
     <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall</t>
   </si>
   <si>
     <t xml:space="preserve">C1: Hazardous Alcohol
@@ -55,6 +58,9 @@
     <t xml:space="preserve"/>
   </si>
   <si>
+    <t xml:space="preserve">**39680**</t>
+  </si>
+  <si>
     <t xml:space="preserve">**5185**</t>
   </si>
   <si>
@@ -100,6 +106,9 @@
     <t xml:space="preserve">Mixta</t>
   </si>
   <si>
+    <t xml:space="preserve"> 3862 ( 9.7) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  669 (12.9) </t>
   </si>
   <si>
@@ -121,6 +130,9 @@
     <t xml:space="preserve">Rural</t>
   </si>
   <si>
+    <t xml:space="preserve"> 2778 ( 7.0) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  560 (10.8) </t>
   </si>
   <si>
@@ -139,6 +151,9 @@
     <t xml:space="preserve">Urbana</t>
   </si>
   <si>
+    <t xml:space="preserve">33040 (83.3) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 3956 (76.3) </t>
   </si>
   <si>
@@ -160,6 +175,9 @@
     <t xml:space="preserve">Without physical comorbidity</t>
   </si>
   <si>
+    <t xml:space="preserve">14982 (37.8) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1952 (37.6) </t>
   </si>
   <si>
@@ -181,6 +199,9 @@
     <t xml:space="preserve">Diagnosis unknown (under study)</t>
   </si>
   <si>
+    <t xml:space="preserve">22550 (56.8) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2956 (57.0) </t>
   </si>
   <si>
@@ -199,6 +220,9 @@
     <t xml:space="preserve">One or more</t>
   </si>
   <si>
+    <t xml:space="preserve"> 2148 ( 5.4) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  277 ( 5.3) </t>
   </si>
   <si>
@@ -217,6 +241,9 @@
     <t xml:space="preserve">edad_b_ap_top_num (median [IQR])</t>
   </si>
   <si>
+    <t xml:space="preserve">32.64 [26.75, 39.25]</t>
+  </si>
+  <si>
     <t xml:space="preserve">35.47 [29.07, 43.04]</t>
   </si>
   <si>
@@ -238,6 +265,9 @@
     <t xml:space="preserve">comorbidity_icd_10 (%)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 8465 (21.3) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  895 (17.3) </t>
   </si>
   <si>
@@ -259,6 +289,9 @@
     <t xml:space="preserve">One</t>
   </si>
   <si>
+    <t xml:space="preserve">16332 (41.2) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2116 (40.8) </t>
   </si>
   <si>
@@ -277,6 +310,9 @@
     <t xml:space="preserve">Two or more</t>
   </si>
   <si>
+    <t xml:space="preserve">  808 ( 2.0) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   93 ( 1.8) </t>
   </si>
   <si>
@@ -295,6 +331,9 @@
     <t xml:space="preserve">Without psychiatric comorbidity</t>
   </si>
   <si>
+    <t xml:space="preserve">14075 (35.5) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2081 (40.1) </t>
   </si>
   <si>
@@ -316,6 +355,9 @@
     <t xml:space="preserve">Alone</t>
   </si>
   <si>
+    <t xml:space="preserve"> 3337 ( 8.4) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  526 (10.1) </t>
   </si>
   <si>
@@ -337,6 +379,9 @@
     <t xml:space="preserve">Family of origin</t>
   </si>
   <si>
+    <t xml:space="preserve">18217 (45.9) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2019 (38.9) </t>
   </si>
   <si>
@@ -352,6 +397,9 @@
     <t xml:space="preserve">Others</t>
   </si>
   <si>
+    <t xml:space="preserve"> 3520 ( 8.9) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  400 ( 7.7) </t>
   </si>
   <si>
@@ -370,6 +418,9 @@
     <t xml:space="preserve">With couple/children</t>
   </si>
   <si>
+    <t xml:space="preserve">14606 (36.8) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2240 (43.2) </t>
   </si>
   <si>
@@ -391,6 +442,9 @@
     <t xml:space="preserve">Alcohol</t>
   </si>
   <si>
+    <t xml:space="preserve">21988 (55.4) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 4302 (83.0) </t>
   </si>
   <si>
@@ -412,6 +466,9 @@
     <t xml:space="preserve">Cocaína</t>
   </si>
   <si>
+    <t xml:space="preserve"> 1512 ( 3.8) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   71 ( 1.4) </t>
   </si>
   <si>
@@ -430,6 +487,9 @@
     <t xml:space="preserve">Marihuana</t>
   </si>
   <si>
+    <t xml:space="preserve">13855 (34.9) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  693 (13.4) </t>
   </si>
   <si>
@@ -448,6 +508,9 @@
     <t xml:space="preserve">Otros</t>
   </si>
   <si>
+    <t xml:space="preserve">  647 ( 1.6) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   44 ( 0.8) </t>
   </si>
   <si>
@@ -466,6 +529,9 @@
     <t xml:space="preserve">Pasta Base</t>
   </si>
   <si>
+    <t xml:space="preserve"> 1549 ( 3.9) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   50 ( 1.0) </t>
   </si>
   <si>
@@ -484,6 +550,9 @@
     <t xml:space="preserve">[Missing]</t>
   </si>
   <si>
+    <t xml:space="preserve">  129 ( 0.3) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   25 ( 0.5) </t>
   </si>
   <si>
@@ -505,6 +574,9 @@
     <t xml:space="preserve">Married/Shared living arrangements</t>
   </si>
   <si>
+    <t xml:space="preserve">12022 (30.3) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1876 (36.2) </t>
   </si>
   <si>
@@ -526,6 +598,9 @@
     <t xml:space="preserve">Separated/Divorced</t>
   </si>
   <si>
+    <t xml:space="preserve"> 3401 ( 8.6) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  543 (10.5) </t>
   </si>
   <si>
@@ -544,6 +619,9 @@
     <t xml:space="preserve">Single</t>
   </si>
   <si>
+    <t xml:space="preserve">23960 (60.4) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2717 (52.4) </t>
   </si>
   <si>
@@ -562,6 +640,9 @@
     <t xml:space="preserve">Widower</t>
   </si>
   <si>
+    <t xml:space="preserve">  249 ( 0.6) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   38 ( 0.7) </t>
   </si>
   <si>
@@ -577,6 +658,9 @@
     <t xml:space="preserve">   20 ( 0.6) </t>
   </si>
   <si>
+    <t xml:space="preserve">   48 ( 0.1) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   11 ( 0.2) </t>
   </si>
   <si>
@@ -598,6 +682,9 @@
     <t xml:space="preserve">1-Mild</t>
   </si>
   <si>
+    <t xml:space="preserve"> 2784 ( 7.0) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  703 (13.6) </t>
   </si>
   <si>
@@ -619,6 +706,9 @@
     <t xml:space="preserve">2-Moderate</t>
   </si>
   <si>
+    <t xml:space="preserve">22773 (57.4) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 3612 (69.7) </t>
   </si>
   <si>
@@ -637,6 +727,9 @@
     <t xml:space="preserve">3-Severe</t>
   </si>
   <si>
+    <t xml:space="preserve">13382 (33.7) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  756 (14.6) </t>
   </si>
   <si>
@@ -652,6 +745,9 @@
     <t xml:space="preserve">  475 (14.4) </t>
   </si>
   <si>
+    <t xml:space="preserve">  741 ( 1.9) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  114 ( 2.2) </t>
   </si>
   <si>
@@ -673,6 +769,9 @@
     <t xml:space="preserve">Center</t>
   </si>
   <si>
+    <t xml:space="preserve">30550 (77.0) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 3768 (72.7) </t>
   </si>
   <si>
@@ -694,6 +793,9 @@
     <t xml:space="preserve">North</t>
   </si>
   <si>
+    <t xml:space="preserve"> 6295 (15.9) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  687 (13.2) </t>
   </si>
   <si>
@@ -712,6 +814,9 @@
     <t xml:space="preserve">South</t>
   </si>
   <si>
+    <t xml:space="preserve"> 2825 ( 7.1) </t>
+  </si>
+  <si>
     <t xml:space="preserve">  728 (14.0) </t>
   </si>
   <si>
@@ -727,6 +832,9 @@
     <t xml:space="preserve">  196 ( 5.9) </t>
   </si>
   <si>
+    <t xml:space="preserve">   10 ( 0.0) </t>
+  </si>
+  <si>
     <t xml:space="preserve">    2 ( 0.0) </t>
   </si>
   <si>
@@ -745,6 +853,9 @@
     <t xml:space="preserve">1-More than high school</t>
   </si>
   <si>
+    <t xml:space="preserve"> 7101 (17.9) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1090 (21.0) </t>
   </si>
   <si>
@@ -766,6 +877,9 @@
     <t xml:space="preserve">2-Completed high school or less</t>
   </si>
   <si>
+    <t xml:space="preserve">22804 (57.5) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2866 (55.3) </t>
   </si>
   <si>
@@ -784,6 +898,9 @@
     <t xml:space="preserve">3-Completed primary school or less</t>
   </si>
   <si>
+    <t xml:space="preserve"> 9656 (24.3) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1202 (23.2) </t>
   </si>
   <si>
@@ -799,6 +916,9 @@
     <t xml:space="preserve">  743 (22.5) </t>
   </si>
   <si>
+    <t xml:space="preserve">  119 ( 0.3) </t>
+  </si>
+  <si>
     <t xml:space="preserve">   27 ( 0.5) </t>
   </si>
   <si>
@@ -820,6 +940,9 @@
     <t xml:space="preserve">Completion</t>
   </si>
   <si>
+    <t xml:space="preserve"> 7461 (18.8) </t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1241 (23.9) </t>
   </si>
   <si>
@@ -839,6 +962,9 @@
   </si>
   <si>
     <t xml:space="preserve">Non-completion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32219 (81.2) </t>
   </si>
   <si>
     <t xml:space="preserve"> 3944 (76.1) </t>
@@ -1216,1349 +1342,1478 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>71</v>
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J15" t="s">
-        <v>104</v>
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="G16" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J16" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J17" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="E18" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J18" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="H19" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J19" t="s">
-        <v>129</v>
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="F20" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="G20" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="D21" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="F21" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J21" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K21" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="E22" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="F22" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="G22" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J22" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="E23" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="G23" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J23" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="E24" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F24" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="G24" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J24" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K24" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="B25" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="F25" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="G25" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="H25" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J25" t="s">
-        <v>167</v>
+        <v>12</v>
+      </c>
+      <c r="K25" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="C26" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="D26" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="E26" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="F26" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="G26" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>198</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J26" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="B27" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="C27" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="D27" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="F27" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="G27" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="D28" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="E28" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="F28" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="G28" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="I28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J28" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="D29" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="E29" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="F29" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="G29" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>218</v>
       </c>
       <c r="I29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J29" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K29" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B30" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="D30" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="E30" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="F30" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="G30" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="H30" t="s">
-        <v>22</v>
+        <v>226</v>
       </c>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J30" t="s">
-        <v>198</v>
+        <v>12</v>
+      </c>
+      <c r="K30" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="C31" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="E31" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="F31" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
       <c r="G31" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>234</v>
       </c>
       <c r="I31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J31" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B32" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="C32" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="D32" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="E32" t="s">
-        <v>208</v>
+        <v>238</v>
       </c>
       <c r="F32" t="s">
-        <v>209</v>
+        <v>239</v>
       </c>
       <c r="G32" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="H32" t="s">
-        <v>11</v>
+        <v>241</v>
       </c>
       <c r="I32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J32" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>211</v>
+        <v>242</v>
       </c>
       <c r="D33" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="E33" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="F33" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
       <c r="G33" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="H33" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="I33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J33" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K33" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>249</v>
       </c>
       <c r="C34" t="s">
-        <v>218</v>
+        <v>250</v>
       </c>
       <c r="D34" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="E34" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="F34" t="s">
-        <v>221</v>
+        <v>253</v>
       </c>
       <c r="G34" t="s">
-        <v>222</v>
+        <v>254</v>
       </c>
       <c r="H34" t="s">
-        <v>22</v>
+        <v>255</v>
       </c>
       <c r="I34" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J34" t="s">
-        <v>223</v>
+        <v>12</v>
+      </c>
+      <c r="K34" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="B35" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="C35" t="s">
-        <v>225</v>
+        <v>258</v>
       </c>
       <c r="D35" t="s">
-        <v>226</v>
+        <v>259</v>
       </c>
       <c r="E35" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="F35" t="s">
-        <v>228</v>
+        <v>261</v>
       </c>
       <c r="G35" t="s">
-        <v>229</v>
+        <v>262</v>
       </c>
       <c r="H35" t="s">
-        <v>11</v>
+        <v>263</v>
       </c>
       <c r="I35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J35" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="B36" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
       <c r="C36" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
       <c r="D36" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="E36" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="F36" t="s">
-        <v>234</v>
+        <v>268</v>
       </c>
       <c r="G36" t="s">
-        <v>235</v>
+        <v>269</v>
       </c>
       <c r="H36" t="s">
-        <v>11</v>
+        <v>270</v>
       </c>
       <c r="I36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J36" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K36" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="B37" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c r="D37" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
       <c r="E37" t="s">
-        <v>236</v>
+        <v>273</v>
       </c>
       <c r="F37" t="s">
-        <v>238</v>
+        <v>272</v>
       </c>
       <c r="G37" t="s">
-        <v>239</v>
+        <v>274</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
+        <v>275</v>
       </c>
       <c r="I37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J37" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K37" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
       <c r="C38" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
       <c r="D38" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
       <c r="E38" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="F38" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
       <c r="G38" t="s">
-        <v>246</v>
+        <v>282</v>
       </c>
       <c r="H38" t="s">
-        <v>22</v>
+        <v>283</v>
       </c>
       <c r="I38" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J38" t="s">
-        <v>247</v>
+        <v>12</v>
+      </c>
+      <c r="K38" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="C39" t="s">
-        <v>249</v>
+        <v>286</v>
       </c>
       <c r="D39" t="s">
-        <v>250</v>
+        <v>287</v>
       </c>
       <c r="E39" t="s">
-        <v>251</v>
+        <v>288</v>
       </c>
       <c r="F39" t="s">
-        <v>252</v>
+        <v>289</v>
       </c>
       <c r="G39" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="H39" t="s">
-        <v>11</v>
+        <v>291</v>
       </c>
       <c r="I39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J39" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K39" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="B40" t="s">
-        <v>254</v>
+        <v>292</v>
       </c>
       <c r="C40" t="s">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="D40" t="s">
-        <v>256</v>
+        <v>294</v>
       </c>
       <c r="E40" t="s">
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="F40" t="s">
-        <v>258</v>
+        <v>296</v>
       </c>
       <c r="G40" t="s">
-        <v>259</v>
+        <v>297</v>
       </c>
       <c r="H40" t="s">
-        <v>11</v>
+        <v>298</v>
       </c>
       <c r="I40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J40" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K40" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
       <c r="D41" t="s">
-        <v>261</v>
+        <v>300</v>
       </c>
       <c r="E41" t="s">
-        <v>262</v>
+        <v>301</v>
       </c>
       <c r="F41" t="s">
-        <v>263</v>
+        <v>302</v>
       </c>
       <c r="G41" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="H41" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="I41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J41" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K41" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>305</v>
       </c>
       <c r="B42" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
       <c r="C42" t="s">
-        <v>267</v>
+        <v>307</v>
       </c>
       <c r="D42" t="s">
-        <v>268</v>
+        <v>308</v>
       </c>
       <c r="E42" t="s">
-        <v>269</v>
+        <v>309</v>
       </c>
       <c r="F42" t="s">
-        <v>270</v>
+        <v>310</v>
       </c>
       <c r="G42" t="s">
-        <v>271</v>
+        <v>311</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>312</v>
       </c>
       <c r="I42" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J42" t="s">
-        <v>272</v>
+        <v>12</v>
+      </c>
+      <c r="K42" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>265</v>
+        <v>305</v>
       </c>
       <c r="B43" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="C43" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="D43" t="s">
-        <v>275</v>
+        <v>316</v>
       </c>
       <c r="E43" t="s">
-        <v>276</v>
+        <v>317</v>
       </c>
       <c r="F43" t="s">
-        <v>277</v>
+        <v>318</v>
       </c>
       <c r="G43" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
       <c r="H43" t="s">
-        <v>11</v>
+        <v>320</v>
       </c>
       <c r="I43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J43" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="K43" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>